<commit_message>
updated source code path
</commit_message>
<xml_diff>
--- a/Paylocity Bugs.xlsx
+++ b/Paylocity Bugs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="0" windowWidth="51200" windowHeight="28340" tabRatio="500"/>
+    <workbookView xWindow="-51200" yWindow="-460" windowWidth="51200" windowHeight="28800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Bugs" sheetId="1" r:id="rId1"/>
@@ -1108,7 +1108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>

</xml_diff>